<commit_message>
Updating LogBook and BurntDownChart
</commit_message>
<xml_diff>
--- a/src/BurntDownChart.xlsx
+++ b/src/BurntDownChart.xlsx
@@ -338,17 +338,6 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -398,6 +387,17 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -513,7 +513,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -543,7 +542,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -553,14 +551,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -570,14 +565,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -587,14 +579,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -604,14 +593,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -621,14 +607,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -638,14 +621,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -655,14 +635,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -672,14 +649,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -689,14 +663,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -706,14 +677,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -723,14 +691,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -740,14 +705,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -757,9 +719,7 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -853,7 +813,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -863,14 +822,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -880,14 +836,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -897,14 +850,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -914,14 +864,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -931,14 +878,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -948,14 +892,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -965,14 +906,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -982,14 +920,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -999,14 +934,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1016,14 +948,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1033,14 +962,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1050,14 +976,11 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1067,9 +990,7 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1123,19 +1044,19 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1190,11 +1111,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="250579744"/>
-        <c:axId val="250580136"/>
+        <c:axId val="259594824"/>
+        <c:axId val="259592472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="250579744"/>
+        <c:axId val="259594824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1132,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="250580136"/>
+        <c:crossAx val="259592472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1219,7 +1140,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="250580136"/>
+        <c:axId val="259592472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1150,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="250579744"/>
+        <c:crossAx val="259594824"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1244,7 +1165,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1661,7 +1581,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,1426 +1593,1420 @@
     <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:19" s="4" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D3" s="2" t="s">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>41785</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>41786</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="4">
         <v>41787</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="4">
         <v>41788</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <v>41789</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="4">
         <v>41790</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="4">
         <v>41792</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>41793</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="4">
         <v>41794</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="4">
         <v>41795</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="4">
         <v>41796</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="4">
         <v>41797</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9">
+      <c r="D6" s="5"/>
+      <c r="E6" s="6">
         <v>3</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
         <f t="shared" ref="I6:Q6" si="0">IF(H6=0,0,H6)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9">
-        <v>2</v>
-      </c>
-      <c r="F7" s="10">
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
         <f t="shared" ref="I7:Q7" si="1">IF(H7=0,0,H7)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9">
+      <c r="D8" s="5"/>
+      <c r="E8" s="6">
         <v>3</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
         <f t="shared" ref="I8:Q8" si="2">IF(H8=0,0,H8)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6">
         <v>4</v>
       </c>
-      <c r="F9" s="9">
-        <v>2</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
         <f t="shared" ref="I9:Q9" si="3">IF(H9=0,0,H9)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P9" s="9">
+      <c r="P9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9">
-        <v>6</v>
-      </c>
-      <c r="F10" s="9">
-        <v>6</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="D10" s="5"/>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="6">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6">
         <v>5</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="6">
         <v>1</v>
       </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
         <f t="shared" ref="J10:Q10" si="4">IF(I10=0,0,I10)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9">
-        <v>6</v>
-      </c>
-      <c r="F11" s="9">
-        <v>6</v>
-      </c>
-      <c r="G11" s="9">
-        <v>6</v>
-      </c>
-      <c r="H11" s="9">
-        <v>6</v>
-      </c>
-      <c r="I11" s="9">
+      <c r="D11" s="5"/>
+      <c r="E11" s="6">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6">
+        <v>6</v>
+      </c>
+      <c r="H11" s="6">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6">
         <v>3</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="6">
         <f>IF(I11=0,0,I11)</f>
         <v>3</v>
       </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" ref="L11:Q25" si="5">IF(K11=0,0,K11)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
+      <c r="M11" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9">
-        <v>6</v>
-      </c>
-      <c r="F12" s="4">
-        <v>6</v>
-      </c>
-      <c r="G12" s="9">
-        <v>6</v>
-      </c>
-      <c r="H12" s="9">
-        <v>6</v>
-      </c>
-      <c r="I12" s="9">
+      <c r="D12" s="5"/>
+      <c r="E12" s="6">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="6">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6</v>
+      </c>
+      <c r="I12" s="6">
         <v>3</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="6">
         <f>IF(I12=0,0,I12)</f>
         <v>3</v>
       </c>
-      <c r="K12" s="9">
-        <v>0</v>
-      </c>
-      <c r="L12" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9">
-        <v>6</v>
-      </c>
-      <c r="F13" s="9">
-        <v>6</v>
-      </c>
-      <c r="G13" s="9">
-        <v>6</v>
-      </c>
-      <c r="H13" s="9">
-        <v>6</v>
-      </c>
-      <c r="I13" s="9">
+      <c r="D13" s="5"/>
+      <c r="E13" s="6">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6">
+        <v>6</v>
+      </c>
+      <c r="H13" s="6">
+        <v>6</v>
+      </c>
+      <c r="I13" s="6">
         <v>3</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="6">
         <f>IF(I13=0,0,I13)</f>
         <v>3</v>
       </c>
-      <c r="K13" s="9">
-        <v>0</v>
-      </c>
-      <c r="L13" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9">
-        <v>6</v>
-      </c>
-      <c r="F14" s="4">
-        <v>6</v>
-      </c>
-      <c r="G14" s="9">
-        <v>6</v>
-      </c>
-      <c r="H14" s="9">
-        <v>6</v>
-      </c>
-      <c r="I14" s="9">
+      <c r="D14" s="5"/>
+      <c r="E14" s="6">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6</v>
+      </c>
+      <c r="G14" s="6">
+        <v>6</v>
+      </c>
+      <c r="H14" s="6">
+        <v>6</v>
+      </c>
+      <c r="I14" s="6">
         <v>3</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="6">
         <v>1</v>
       </c>
-      <c r="K14" s="9">
-        <v>0</v>
-      </c>
-      <c r="L14" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9">
-        <v>6</v>
-      </c>
-      <c r="F15" s="10">
-        <v>6</v>
-      </c>
-      <c r="G15" s="9">
-        <v>6</v>
-      </c>
-      <c r="H15" s="9">
-        <v>6</v>
-      </c>
-      <c r="I15" s="9">
+      <c r="D15" s="5"/>
+      <c r="E15" s="6">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7">
+        <v>6</v>
+      </c>
+      <c r="G15" s="6">
+        <v>6</v>
+      </c>
+      <c r="H15" s="6">
+        <v>6</v>
+      </c>
+      <c r="I15" s="6">
         <f t="shared" ref="I15:K25" si="6">IF(H15=0,0,H15)</f>
         <v>6</v>
       </c>
-      <c r="J15" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K15" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L15" s="9">
+      <c r="J15" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L15" s="6">
         <v>4</v>
       </c>
-      <c r="M15" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="N15" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="O15" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P15" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="Q15" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="M15" s="6">
+        <v>2</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P15" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q15" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9">
-        <v>6</v>
-      </c>
-      <c r="F16" s="10">
-        <v>6</v>
-      </c>
-      <c r="G16" s="9">
-        <v>6</v>
-      </c>
-      <c r="H16" s="9">
-        <v>6</v>
-      </c>
-      <c r="I16" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J16" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K16" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L16" s="9">
+      <c r="D16" s="5"/>
+      <c r="E16" s="6">
+        <v>6</v>
+      </c>
+      <c r="F16" s="7">
+        <v>6</v>
+      </c>
+      <c r="G16" s="6">
+        <v>6</v>
+      </c>
+      <c r="H16" s="6">
+        <v>6</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L16" s="6">
         <v>4</v>
       </c>
-      <c r="M16" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="N16" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="O16" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P16" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="Q16" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+      <c r="M16" s="6">
+        <v>2</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P16" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q16" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9">
-        <v>6</v>
-      </c>
-      <c r="F17" s="9">
-        <v>6</v>
-      </c>
-      <c r="G17" s="9">
-        <v>6</v>
-      </c>
-      <c r="H17" s="9">
-        <v>6</v>
-      </c>
-      <c r="I17" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J17" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K17" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L17" s="9">
+      <c r="D17" s="5"/>
+      <c r="E17" s="6">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6">
+        <v>6</v>
+      </c>
+      <c r="H17" s="6">
+        <v>6</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L17" s="6">
         <v>4</v>
       </c>
-      <c r="M17" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="N17" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="O17" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P17" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="Q17" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
+      <c r="M17" s="6">
+        <v>2</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P17" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q17" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10">
-        <v>6</v>
-      </c>
-      <c r="F18" s="12">
-        <v>6</v>
-      </c>
-      <c r="G18" s="10">
-        <v>6</v>
-      </c>
-      <c r="H18" s="9">
-        <v>6</v>
-      </c>
-      <c r="I18" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J18" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K18" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L18" s="9">
+      <c r="D18" s="8"/>
+      <c r="E18" s="7">
+        <v>6</v>
+      </c>
+      <c r="F18" s="9">
+        <v>6</v>
+      </c>
+      <c r="G18" s="7">
+        <v>6</v>
+      </c>
+      <c r="H18" s="6">
+        <v>6</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L18" s="6">
         <v>4</v>
       </c>
-      <c r="M18" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="N18" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="O18" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P18" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="Q18" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
+      <c r="M18" s="6">
+        <v>2</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10">
-        <v>6</v>
-      </c>
-      <c r="F19" s="12">
-        <v>6</v>
-      </c>
-      <c r="G19" s="10">
-        <v>6</v>
-      </c>
-      <c r="H19" s="9">
-        <v>6</v>
-      </c>
-      <c r="I19" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J19" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K19" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L19" s="9">
+      <c r="D19" s="8"/>
+      <c r="E19" s="7">
+        <v>6</v>
+      </c>
+      <c r="F19" s="9">
+        <v>6</v>
+      </c>
+      <c r="G19" s="7">
+        <v>6</v>
+      </c>
+      <c r="H19" s="6">
+        <v>6</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L19" s="6">
         <v>4</v>
       </c>
-      <c r="M19" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="N19" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="O19" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P19" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="Q19" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
+      <c r="M19" s="6">
+        <v>2</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q19" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="14" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="9">
-        <v>6</v>
-      </c>
-      <c r="F20" s="16">
-        <v>6</v>
-      </c>
-      <c r="G20" s="9">
-        <v>6</v>
-      </c>
-      <c r="H20" s="9">
-        <v>6</v>
-      </c>
-      <c r="I20" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J20" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K20" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L20" s="9">
+      <c r="D20" s="12"/>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+      <c r="F20" s="13">
+        <v>6</v>
+      </c>
+      <c r="G20" s="6">
+        <v>6</v>
+      </c>
+      <c r="H20" s="6">
+        <v>6</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L20" s="6">
         <v>4</v>
       </c>
-      <c r="M20" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="N20" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="O20" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P20" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="Q20" s="9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+      <c r="M20" s="6">
+        <v>2</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P20" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q20" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19">
-        <v>6</v>
-      </c>
-      <c r="F21" s="20">
-        <v>6</v>
-      </c>
-      <c r="G21" s="19">
-        <v>6</v>
-      </c>
-      <c r="H21" s="9">
-        <v>6</v>
-      </c>
-      <c r="I21" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J21" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K21" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L21" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="M21" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="N21" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="O21" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P21" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="Q21" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16">
+        <v>6</v>
+      </c>
+      <c r="F21" s="17">
+        <v>6</v>
+      </c>
+      <c r="G21" s="16">
+        <v>6</v>
+      </c>
+      <c r="H21" s="6">
+        <v>6</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="M21" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P21" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="Q21" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="9">
-        <v>6</v>
-      </c>
-      <c r="F22" s="16">
-        <v>6</v>
-      </c>
-      <c r="G22" s="9">
-        <v>6</v>
-      </c>
-      <c r="H22" s="9">
-        <v>6</v>
-      </c>
-      <c r="I22" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J22" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K22" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L22" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="M22" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="N22" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="O22" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P22" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="Q22" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="6">
+        <v>6</v>
+      </c>
+      <c r="F22" s="13">
+        <v>6</v>
+      </c>
+      <c r="G22" s="6">
+        <v>6</v>
+      </c>
+      <c r="H22" s="6">
+        <v>6</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="M22" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N22" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P22" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="Q22" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19">
-        <v>6</v>
-      </c>
-      <c r="F23" s="20">
-        <v>6</v>
-      </c>
-      <c r="G23" s="19">
-        <v>6</v>
-      </c>
-      <c r="H23" s="9">
-        <v>6</v>
-      </c>
-      <c r="I23" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J23" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K23" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L23" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="M23" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="N23" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="O23" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P23" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="Q23" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16">
+        <v>6</v>
+      </c>
+      <c r="F23" s="17">
+        <v>6</v>
+      </c>
+      <c r="G23" s="16">
+        <v>6</v>
+      </c>
+      <c r="H23" s="6">
+        <v>6</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="M23" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N23" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O23" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P23" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="Q23" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="14" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="9">
-        <v>6</v>
-      </c>
-      <c r="F24" s="16">
-        <v>6</v>
-      </c>
-      <c r="G24" s="9">
-        <v>6</v>
-      </c>
-      <c r="H24" s="9">
-        <v>6</v>
-      </c>
-      <c r="I24" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="J24" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="K24" s="9">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="L24" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="M24" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="N24" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="O24" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P24" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="Q24" s="9">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="6">
+        <v>6</v>
+      </c>
+      <c r="F24" s="13">
+        <v>6</v>
+      </c>
+      <c r="G24" s="6">
+        <v>6</v>
+      </c>
+      <c r="H24" s="6">
+        <v>6</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N24" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P24" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="Q24" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9">
-        <v>2</v>
-      </c>
-      <c r="F25" s="10">
-        <v>2</v>
-      </c>
-      <c r="G25" s="9">
-        <v>2</v>
-      </c>
-      <c r="H25" s="9">
-        <v>2</v>
-      </c>
-      <c r="I25" s="9">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="J25" s="9">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="K25" s="9">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L25" s="9">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M25" s="9">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N25" s="9">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O25" s="9">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P25" s="9">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q25" s="9">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6">
+        <v>2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>2</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2</v>
+      </c>
+      <c r="H25" s="6">
+        <v>2</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N25" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P25" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q25" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="9">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="6">
         <f>SUM(E6:E25)</f>
         <v>104</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="7">
         <f t="shared" ref="F26:P26" si="7">ROUND(E26-$E$26/12,0)</f>
         <v>95</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="7">
         <f t="shared" si="7"/>
         <v>86</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="7">
         <f t="shared" si="7"/>
         <v>77</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="7">
         <f t="shared" si="7"/>
         <v>68</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="7">
         <f t="shared" si="7"/>
         <v>59</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="7">
         <f t="shared" si="7"/>
         <v>50</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="7">
         <f t="shared" si="7"/>
         <v>41</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="7">
         <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="N26" s="10">
+      <c r="N26" s="7">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26" s="7">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="P26" s="10">
+      <c r="P26" s="7">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="Q26" s="10">
-        <v>0</v>
-      </c>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="Q26" s="7">
+        <v>0</v>
+      </c>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="9">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="6">
         <f t="shared" ref="E27:Q27" si="8">SUM(E6:E25)</f>
         <v>104</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="6">
         <f t="shared" si="8"/>
         <v>97</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="6">
         <f t="shared" si="8"/>
         <v>91</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="6">
         <f t="shared" si="8"/>
         <v>87</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="6">
         <f t="shared" si="8"/>
         <v>74</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="6">
         <f t="shared" si="8"/>
         <v>72</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="6">
         <f t="shared" si="8"/>
         <v>62</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="6">
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="6">
         <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="N27" s="9">
+        <v>38</v>
+      </c>
+      <c r="N27" s="6">
         <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="O27" s="9">
+        <v>38</v>
+      </c>
+      <c r="O27" s="6">
         <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="P27" s="9">
+        <v>38</v>
+      </c>
+      <c r="P27" s="6">
         <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="Q27" s="9">
+        <v>38</v>
+      </c>
+      <c r="Q27" s="6">
         <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
     </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
update LogBVook dan BurntDownChart
</commit_message>
<xml_diff>
--- a/src/BurntDownChart.xlsx
+++ b/src/BurntDownChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Presentasi-TKPPL\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GianGaeL\Documents\GitHub\Presentasi-TKPPL\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -513,6 +513,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -542,6 +543,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -551,11 +553,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -565,11 +570,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -579,11 +587,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -593,11 +604,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -607,11 +621,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -621,11 +638,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -635,11 +655,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -649,11 +672,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -663,11 +689,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -677,11 +706,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -691,11 +723,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -705,11 +740,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -719,7 +757,9 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -813,6 +853,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -822,11 +863,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -836,11 +880,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -850,11 +897,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -864,11 +914,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -878,11 +931,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -892,11 +948,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -906,11 +965,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -920,11 +982,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -934,11 +999,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -948,11 +1016,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -962,11 +1033,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -976,11 +1050,14 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
+              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -990,7 +1067,9 @@
               <c:showBubbleSize val="1"/>
               <c:separator>; </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1050,13 +1129,13 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1111,11 +1190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="235822728"/>
-        <c:axId val="235825864"/>
+        <c:axId val="206612000"/>
+        <c:axId val="206607296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="235822728"/>
+        <c:axId val="206612000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1211,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="235825864"/>
+        <c:crossAx val="206607296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1140,7 +1219,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235825864"/>
+        <c:axId val="206607296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,7 +1229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="235822728"/>
+        <c:crossAx val="206612000"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1165,6 +1244,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1580,8 +1660,8 @@
   </sheetPr>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,16 +2684,15 @@
         <v>6</v>
       </c>
       <c r="O21" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P21" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q21" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2664,16 +2743,15 @@
         <v>6</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P22" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q22" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2724,16 +2802,15 @@
         <v>6</v>
       </c>
       <c r="O23" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P23" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q23" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2784,16 +2861,15 @@
         <v>6</v>
       </c>
       <c r="O24" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P24" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q24" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2844,16 +2920,15 @@
         <v>2</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P25" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -2968,15 +3043,15 @@
       </c>
       <c r="O27" s="6">
         <f t="shared" si="8"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P27" s="6">
         <f t="shared" si="8"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Q27" s="6">
         <f t="shared" si="8"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>

</xml_diff>

<commit_message>
update logbook & burnt down chart
</commit_message>
<xml_diff>
--- a/src/BurntDownChart.xlsx
+++ b/src/BurntDownChart.xlsx
@@ -1132,10 +1132,10 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1190,11 +1190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206612000"/>
-        <c:axId val="206607296"/>
+        <c:axId val="212996656"/>
+        <c:axId val="212992344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206612000"/>
+        <c:axId val="212996656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1211,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="206607296"/>
+        <c:crossAx val="212992344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1219,7 +1219,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206607296"/>
+        <c:axId val="212992344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="206612000"/>
+        <c:crossAx val="212996656"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1660,8 +1660,8 @@
   </sheetPr>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,12 +2687,11 @@
         <v>4</v>
       </c>
       <c r="P21" s="6">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q21" s="6">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2746,12 +2745,11 @@
         <v>4</v>
       </c>
       <c r="P22" s="6">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="6">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2805,12 +2803,11 @@
         <v>4</v>
       </c>
       <c r="P23" s="6">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="6">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2864,12 +2861,11 @@
         <v>4</v>
       </c>
       <c r="P24" s="6">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q24" s="6">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -3047,11 +3043,11 @@
       </c>
       <c r="P27" s="6">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="Q27" s="6">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>

</xml_diff>